<commit_message>
Added compressor and CPu
</commit_message>
<xml_diff>
--- a/adopt_net0/database/templates/technology_data/Industrial/CementHybridCCS_data/cement_sheet.xlsx
+++ b/adopt_net0/database/templates/technology_data/Industrial/CementHybridCCS_data/cement_sheet.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AdOpT-NET0\adopt_net0\database\templates\technology_data\Industrial\CementHybridCCS_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC3FA7B-B280-4278-B89C-46542FB039ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791A84AB-DAFF-4197-9592-1CBD599E4F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C0ECAA26-0769-408D-9398-31AECF4E3649}"/>
+    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C0ECAA26-0769-408D-9398-31AECF4E3649}"/>
   </bookViews>
   <sheets>
-    <sheet name="oxyfuel" sheetId="1" r:id="rId1"/>
-    <sheet name="mea" sheetId="2" r:id="rId2"/>
-    <sheet name="other_data" sheetId="3" r:id="rId3"/>
-    <sheet name="calculations" sheetId="4" r:id="rId4"/>
+    <sheet name="capex_oxyfuel" sheetId="1" r:id="rId1"/>
+    <sheet name="capex_mea" sheetId="2" r:id="rId2"/>
+    <sheet name="capex_cpu_oxyfuel" sheetId="6" r:id="rId3"/>
+    <sheet name="capex_compressor_mea" sheetId="5" r:id="rId4"/>
+    <sheet name="energy_oxy_mea" sheetId="3" r:id="rId5"/>
+    <sheet name="energy_cpu_compressor" sheetId="7" r:id="rId6"/>
+    <sheet name="calculations" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="68">
   <si>
     <t>size_tclinker_per_h</t>
   </si>
@@ -295,6 +298,24 @@
   <si>
     <t>value</t>
   </si>
+  <si>
+    <t>el_cons_cpu</t>
+  </si>
+  <si>
+    <t>electricity_cons_MWh/tCO2</t>
+  </si>
+  <si>
+    <t>liquid</t>
+  </si>
+  <si>
+    <t>gas</t>
+  </si>
+  <si>
+    <t>supercritical</t>
+  </si>
+  <si>
+    <t>el_cons_compressor</t>
+  </si>
 </sst>
 </file>
 
@@ -303,7 +324,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,6 +374,12 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -540,7 +567,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -598,6 +625,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="5" builtinId="22"/>
@@ -940,7 +972,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,11 +1015,12 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1001,7 +1034,8 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>3.75</v>
+        <f>calculations!D15</f>
+        <v>3.7084942228242932</v>
       </c>
       <c r="B2">
         <f>calculations!D16</f>
@@ -1010,7 +1044,8 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12.51</v>
+        <f>calculations!G15</f>
+        <v>12.361647409414312</v>
       </c>
       <c r="B3">
         <f>calculations!G16</f>
@@ -1019,7 +1054,8 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>20.85</v>
+        <f>calculations!G6</f>
+        <v>20.602745682357188</v>
       </c>
       <c r="B4">
         <f>calculations!G7</f>
@@ -1033,11 +1069,156 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DFFB0-96B6-4F96-B3DF-E2D36B37C43F}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>75</v>
+      </c>
+      <c r="B2">
+        <v>48600000</v>
+      </c>
+      <c r="C2">
+        <v>50200000</v>
+      </c>
+      <c r="D2">
+        <v>61000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>125</v>
+      </c>
+      <c r="B3">
+        <v>62500000</v>
+      </c>
+      <c r="C3">
+        <v>63300000</v>
+      </c>
+      <c r="D3">
+        <v>71600000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8995DE27-F5E7-40F1-8502-5CC793EB5921}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>calculations!D15</f>
+        <v>3.7084942228242932</v>
+      </c>
+      <c r="B2">
+        <v>7530000</v>
+      </c>
+      <c r="C2">
+        <f>8.00649089380739*10^6</f>
+        <v>8006490.8938073898</v>
+      </c>
+      <c r="D2">
+        <f>10.684945673991*10^6</f>
+        <v>10684945.673991</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>calculations!G15</f>
+        <v>12.361647409414312</v>
+      </c>
+      <c r="B3">
+        <f>11.2041255209316*10^6</f>
+        <v>11204125.5209316</v>
+      </c>
+      <c r="C3">
+        <f>12.5665678479893*10^6</f>
+        <v>12566567.847989298</v>
+      </c>
+      <c r="D3">
+        <f>16.5887397694844*10^6</f>
+        <v>16588739.769484399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>calculations!G6</f>
+        <v>20.602745682357188</v>
+      </c>
+      <c r="B4">
+        <f>13.2435084663724*10^6</f>
+        <v>13243508.466372401</v>
+      </c>
+      <c r="C4">
+        <f>15.1282369696705*10^6</f>
+        <v>15128236.969670501</v>
+      </c>
+      <c r="D4">
+        <f>19.9398066221897*10^6</f>
+        <v>19939806.622189701</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69712579-C7D8-42EE-9801-1FD637D0A17F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,11 +1260,80 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21185F42-04E5-4941-B133-36036095D1EF}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="26">
+        <v>0.17050594000000002</v>
+      </c>
+      <c r="C2" s="26">
+        <v>0.120245032</v>
+      </c>
+      <c r="D2" s="26">
+        <v>0.13739152500000001</v>
+      </c>
+      <c r="E2" s="25"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="27">
+        <v>0.11930297990344463</v>
+      </c>
+      <c r="C3" s="27">
+        <v>7.4589551950173874E-2</v>
+      </c>
+      <c r="D3" s="27">
+        <v>8.9737128657946114E-2</v>
+      </c>
+      <c r="E3" s="25"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB78D47C-565F-4352-814A-A37F11C35FBF}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -2725,6 +2975,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:B14"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:B5"/>
     <mergeCell ref="C2:G2"/>
@@ -2733,14 +2991,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:B14"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added CAPEX and OPEX of compressor and CPU
</commit_message>
<xml_diff>
--- a/adopt_net0/database/templates/technology_data/Industrial/CementHybridCCS_data/cement_sheet.xlsx
+++ b/adopt_net0/database/templates/technology_data/Industrial/CementHybridCCS_data/cement_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AdOpT-NET0\adopt_net0\database\templates\technology_data\Industrial\CementHybridCCS_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791A84AB-DAFF-4197-9592-1CBD599E4F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1A2A18-7943-4B3D-9E3F-F96EF1E288A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-180" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{C0ECAA26-0769-408D-9398-31AECF4E3649}"/>
+    <workbookView xWindow="22932" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{C0ECAA26-0769-408D-9398-31AECF4E3649}"/>
   </bookViews>
   <sheets>
     <sheet name="capex_oxyfuel" sheetId="1" r:id="rId1"/>
@@ -589,6 +589,11 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -625,11 +630,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="5" builtinId="22"/>
@@ -975,13 +975,13 @@
       <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -989,7 +989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>75</v>
       </c>
@@ -997,7 +997,7 @@
         <v>137540000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>125</v>
       </c>
@@ -1018,13 +1018,13 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>calculations!D15</f>
         <v>3.7084942228242932</v>
@@ -1042,7 +1042,7 @@
         <v>28210000.000000007</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>calculations!G15</f>
         <v>12.361647409414312</v>
@@ -1052,7 +1052,7 @@
         <v>46360000.000000015</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>calculations!G6</f>
         <v>20.602745682357188</v>
@@ -1070,15 +1070,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DFFB0-96B6-4F96-B3DF-E2D36B37C43F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1092,31 +1092,45 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
         <v>75</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>48600000</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>50200000</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <v>61000000</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>125</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>62500000</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>63300000</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>71600000</v>
       </c>
     </row>
@@ -1127,21 +1141,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8995DE27-F5E7-40F1-8502-5CC793EB5921}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -1155,55 +1169,69 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
         <f>calculations!D15</f>
         <v>3.7084942228242932</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>7530000</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <f>8.00649089380739*10^6</f>
         <v>8006490.8938073898</v>
       </c>
-      <c r="D2">
+      <c r="D3">
         <f>10.684945673991*10^6</f>
         <v>10684945.673991</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
         <f>calculations!G15</f>
         <v>12.361647409414312</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <f>11.2041255209316*10^6</f>
         <v>11204125.5209316</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <f>12.5665678479893*10^6</f>
         <v>12566567.847989298</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <f>16.5887397694844*10^6</f>
         <v>16588739.769484399</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
         <f>calculations!G6</f>
         <v>20.602745682357188</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <f>13.2435084663724*10^6</f>
         <v>13243508.466372401</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <f>15.1282369696705*10^6</f>
         <v>15128236.969670501</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <f>19.9398066221897*10^6</f>
         <v>19939806.622189701</v>
       </c>
@@ -1221,14 +1249,14 @@
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1237,7 +1265,7 @@
         <v>0.25548249251013122</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1246,7 +1274,7 @@
         <v>8.2307186539958971E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -1264,16 +1292,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21185F42-04E5-4941-B133-36036095D1EF}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1287,42 +1315,42 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="26">
+      <c r="B2" s="14">
         <v>0.17050594000000002</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="14">
         <v>0.120245032</v>
       </c>
-      <c r="D2" s="26">
+      <c r="D2" s="14">
         <v>0.13739152500000001</v>
       </c>
-      <c r="E2" s="25"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="E2" s="13"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="15">
         <v>0.11930297990344463</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="15">
         <v>7.4589551950173874E-2</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="15">
         <v>8.9737128657946114E-2</v>
       </c>
-      <c r="E3" s="25"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
+      <c r="E3" s="13"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1337,23 +1365,23 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="18"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11" t="s">
         <v>50</v>
@@ -1364,18 +1392,18 @@
       <c r="S1" s="11"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="23"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="26"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3" t="s">
         <v>27</v>
@@ -1396,9 +1424,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="21"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1436,22 +1464,22 @@
         <v>3000.20095584</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="24">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="21"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="27">
         <v>151.62</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="27">
         <v>187.3</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="27">
         <v>195.27</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="27">
         <v>206.45</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="27">
         <v>214.07</v>
       </c>
       <c r="N4" s="3" t="s">
@@ -1476,14 +1504,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="23"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="27"/>
       <c r="N5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1506,7 +1534,7 @@
         <v>31.161112290000002</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" s="7" t="s">
         <v>19</v>
       </c>
@@ -1551,7 +1579,7 @@
         <v>0.29092152256564102</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
@@ -1594,7 +1622,7 @@
         <v>5.708245328833919</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
@@ -1637,7 +1665,7 @@
         <v>30.870190767434362</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1679,16 +1707,16 @@
         <v>28.646099032989916</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A10" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
       <c r="N10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1711,18 +1739,18 @@
         <v>26.42200729854547</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" x14ac:dyDescent="0.35">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
       <c r="N11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1745,9 +1773,9 @@
         <v>0.98994638988464256</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="21"/>
+      <c r="B12" s="22"/>
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
@@ -1785,22 +1813,22 @@
         <v>4.6709789600000002</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="24">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="27">
         <v>137.54</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="27">
         <v>165.75</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="27">
         <v>172.9</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="27">
         <v>179.8</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="27">
         <v>183.9</v>
       </c>
       <c r="N13" s="3" t="s">
@@ -1825,14 +1853,14 @@
         <v>8.5676397800000004</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="23"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
       <c r="N14" s="3" t="s">
         <v>39</v>
       </c>
@@ -1855,7 +1883,7 @@
         <v>24.178772760488858</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="7" t="s">
         <v>19</v>
@@ -1901,7 +1929,7 @@
         <v>4.2357627200000003</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" s="7" t="s">
         <v>24</v>
       </c>
@@ -1944,7 +1972,7 @@
         <v>7.0940057399999992</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
@@ -1987,7 +2015,7 @@
         <v>0.36178175000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>26</v>
       </c>
@@ -2029,7 +2057,7 @@
         <v>54.302358825637938</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N19" s="3" t="s">
         <v>44</v>
       </c>
@@ -2052,7 +2080,7 @@
         <v>1.1158962699999997</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N20" s="3" t="s">
         <v>45</v>
       </c>
@@ -2075,7 +2103,7 @@
         <v>40368.159200000002</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
@@ -2107,7 +2135,7 @@
         <v>-16.189386439511143</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
@@ -2133,7 +2161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>12</v>
       </c>
@@ -2173,7 +2201,7 @@
         <v>0.75061547957059027</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>13</v>
       </c>
@@ -2206,7 +2234,7 @@
         <v>7456.9033862699989</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
         <v>17</v>
       </c>
@@ -2243,7 +2271,7 @@
         <v>67.099101114943267</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>18</v>
       </c>
@@ -2280,7 +2308,7 @@
         <v>8.3779786486448486</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
         <v>23</v>
       </c>
@@ -2313,7 +2341,7 @@
         <v>3652.0872323173585</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>18</v>
       </c>
@@ -2332,7 +2360,7 @@
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
     </row>
-    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>22</v>
       </c>
@@ -2353,7 +2381,7 @@
       <c r="S29" s="11"/>
       <c r="T29" s="11"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N30" s="3"/>
       <c r="O30" s="3" t="s">
         <v>27</v>
@@ -2374,7 +2402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N31" s="3" t="s">
         <v>28</v>
       </c>
@@ -2397,7 +2425,7 @@
         <v>1799.9672083200001</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>54</v>
       </c>
@@ -2430,7 +2458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>55</v>
       </c>
@@ -2463,7 +2491,7 @@
         <v>18.706244290000001</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>56</v>
       </c>
@@ -2496,7 +2524,7 @@
         <v>0.17574765294122172</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N35" s="3" t="s">
         <v>32</v>
       </c>
@@ -2519,7 +2547,7 @@
         <v>3.4278460399999999</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N36" s="3" t="s">
         <v>33</v>
       </c>
@@ -2542,7 +2570,7 @@
         <v>18.530496637058778</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N37" s="3" t="s">
         <v>34</v>
       </c>
@@ -2565,7 +2593,7 @@
         <v>17.185376043221318</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N38" s="3" t="s">
         <v>35</v>
       </c>
@@ -2588,7 +2616,7 @@
         <v>15.840255449383857</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N39" s="3" t="s">
         <v>36</v>
       </c>
@@ -2611,7 +2639,7 @@
         <v>0.98987694252877945</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N40" s="3" t="s">
         <v>37</v>
       </c>
@@ -2634,7 +2662,7 @@
         <v>2.8013522599999998</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N41" s="3" t="s">
         <v>38</v>
       </c>
@@ -2657,7 +2685,7 @@
         <v>5.1205206399999996</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N42" s="3" t="s">
         <v>39</v>
       </c>
@@ -2680,7 +2708,7 @@
         <v>14.573233709896117</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N43" s="3" t="s">
         <v>40</v>
       </c>
@@ -2703,7 +2731,7 @@
         <v>4.2514259799999996</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N44" s="3" t="s">
         <v>41</v>
       </c>
@@ -2726,7 +2754,7 @@
         <v>4.2397910899999998</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N45" s="3" t="s">
         <v>42</v>
       </c>
@@ -2749,7 +2777,7 @@
         <v>0.18547881599999999</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N46" s="3" t="s">
         <v>43</v>
       </c>
@@ -2772,7 +2800,7 @@
         <v>54.474585290604679</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N47" s="3" t="s">
         <v>44</v>
       </c>
@@ -2795,7 +2823,7 @@
         <v>0.67222976928854927</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N48" s="3" t="s">
         <v>45</v>
       </c>
@@ -2818,7 +2846,7 @@
         <v>23737.731500000002</v>
       </c>
     </row>
-    <row r="49" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N49" s="3" t="s">
         <v>46</v>
       </c>
@@ -2841,7 +2869,7 @@
         <v>-9.1644977901038853</v>
       </c>
     </row>
-    <row r="50" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N50" s="3"/>
       <c r="O50" s="12"/>
       <c r="P50" s="12"/>
@@ -2858,7 +2886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N51" s="3" t="s">
         <v>51</v>
       </c>
@@ -2881,7 +2909,7 @@
         <v>0.74863011783778244</v>
       </c>
     </row>
-    <row r="52" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N52" s="3" t="s">
         <v>47</v>
       </c>
@@ -2904,7 +2932,7 @@
         <v>4425.9421357692881</v>
       </c>
     </row>
-    <row r="53" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N53" s="3" t="s">
         <v>52</v>
       </c>
@@ -2927,7 +2955,7 @@
         <v>66.346218081835687</v>
       </c>
     </row>
-    <row r="54" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N54" s="3" t="s">
         <v>48</v>
       </c>
@@ -2950,7 +2978,7 @@
         <v>8.4360410255996303</v>
       </c>
     </row>
-    <row r="55" spans="14:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="14:20" x14ac:dyDescent="0.3">
       <c r="N55" s="3" t="s">
         <v>49</v>
       </c>
@@ -2975,6 +3003,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:B5"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A11:B14"/>
     <mergeCell ref="C11:G11"/>
@@ -2983,14 +3019,6 @@
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="G13:G14"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:B5"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Small change cement sheet
</commit_message>
<xml_diff>
--- a/adopt_net0/database/templates/technology_data/Industrial/CementHybridCCS_data/cement_sheet.xlsx
+++ b/adopt_net0/database/templates/technology_data/Industrial/CementHybridCCS_data/cement_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AdOpT-NET0\adopt_net0\database\templates\technology_data\Industrial\CementHybridCCS_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1A2A18-7943-4B3D-9E3F-F96EF1E288A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02074255-3BE7-4E40-BA27-190CC16F52C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{C0ECAA26-0769-408D-9398-31AECF4E3649}"/>
+    <workbookView xWindow="22932" yWindow="-4404" windowWidth="30936" windowHeight="16896" activeTab="6" xr2:uid="{C0ECAA26-0769-408D-9398-31AECF4E3649}"/>
   </bookViews>
   <sheets>
     <sheet name="capex_oxyfuel" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="72">
   <si>
     <t>size_tclinker_per_h</t>
   </si>
@@ -315,6 +315,18 @@
   </si>
   <si>
     <t>el_cons_compressor</t>
+  </si>
+  <si>
+    <t>fixed OPEX MEUR</t>
+  </si>
+  <si>
+    <t>compressor/cpu supercritical capex MEUR</t>
+  </si>
+  <si>
+    <t>fixed O&amp;M as fraction of capex oxy+cpu</t>
+  </si>
+  <si>
+    <t>fixed O&amp;M as fraction of capex MEA+compressor</t>
   </si>
 </sst>
 </file>
@@ -567,7 +579,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -630,6 +642,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="12" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="13" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="5" builtinId="22"/>
@@ -1034,21 +1055,21 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>calculations!D15</f>
+        <f>calculations!D19</f>
         <v>3.7084942228242932</v>
       </c>
       <c r="B2">
-        <f>calculations!D16</f>
+        <f>calculations!D20</f>
         <v>28210000.000000007</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>calculations!G15</f>
+        <f>calculations!G19</f>
         <v>12.361647409414312</v>
       </c>
       <c r="B3">
-        <f>calculations!G16</f>
+        <f>calculations!G20</f>
         <v>46360000.000000015</v>
       </c>
     </row>
@@ -1072,7 +1093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17DFFB0-96B6-4F96-B3DF-E2D36B37C43F}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1185,7 +1206,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>calculations!D15</f>
+        <f>calculations!D19</f>
         <v>3.7084942228242932</v>
       </c>
       <c r="B3">
@@ -1202,7 +1223,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>calculations!G15</f>
+        <f>calculations!G19</f>
         <v>12.361647409414312</v>
       </c>
       <c r="B4">
@@ -1246,7 +1267,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1261,7 +1282,7 @@
         <v>58</v>
       </c>
       <c r="B2">
-        <f>calculations!C32</f>
+        <f>calculations!C38</f>
         <v>0.25548249251013122</v>
       </c>
     </row>
@@ -1270,7 +1291,7 @@
         <v>59</v>
       </c>
       <c r="B3">
-        <f>calculations!C33</f>
+        <f>calculations!C39</f>
         <v>8.2307186539958971E-2</v>
       </c>
     </row>
@@ -1279,7 +1300,7 @@
         <v>60</v>
       </c>
       <c r="B4">
-        <f>calculations!C34</f>
+        <f>calculations!C40</f>
         <v>5.4302358825637935E-2</v>
       </c>
     </row>
@@ -1293,7 +1314,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1361,14 +1382,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB78D47C-565F-4352-814A-A37F11C35FBF}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1542,19 +1563,19 @@
         <v>0</v>
       </c>
       <c r="D6" s="7">
-        <f>125*$C$25*(1-$C$29)*$C$27*0.3</f>
+        <f>125*$C$31*(1-$C$35)*$C$33*0.3</f>
         <v>6.1808237047071559</v>
       </c>
       <c r="E6" s="7">
-        <f>125*$C$25*(1-$C$29)*$C$27*0.5</f>
+        <f>125*$C$31*(1-$C$35)*$C$33*0.5</f>
         <v>10.301372841178594</v>
       </c>
       <c r="F6" s="7">
-        <f>125*$C$25*(1-$C$29)*$C$27*0.8</f>
+        <f>125*$C$31*(1-$C$35)*$C$33*0.8</f>
         <v>16.482196545885753</v>
       </c>
       <c r="G6" s="7">
-        <f>125*$C$25*(1-$C$29)*$C$27*1</f>
+        <f>125*$C$31*(1-$C$35)*$C$33*1</f>
         <v>20.602745682357188</v>
       </c>
       <c r="N6" s="3" t="s">
@@ -1597,7 +1618,7 @@
         <v>54829999.999999985</v>
       </c>
       <c r="G7" s="7">
-        <f t="shared" si="0"/>
+        <f>(G4-$C$4)*10^6</f>
         <v>62449999.999999985</v>
       </c>
       <c r="N7" s="3" t="s">
@@ -1622,7 +1643,7 @@
         <v>5.708245328833919</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="7" t="s">
         <v>25</v>
       </c>
@@ -1665,7 +1686,7 @@
         <v>30.870190767434362</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>26</v>
       </c>
@@ -1674,15 +1695,15 @@
         <v>5.772693366553562</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:G9" si="2">E8/10^6</f>
+        <f>E8/10^6</f>
         <v>4.237299306895677</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f>F8/10^6</f>
         <v>3.3266197164531763</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f>G8/10^6</f>
         <v>3.0311493896407207</v>
       </c>
       <c r="N9" s="3" t="s">
@@ -1707,16 +1728,25 @@
         <v>28.646099032989916</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="28">
+        <v>10.5</v>
+      </c>
+      <c r="D10" s="28">
+        <v>16.8</v>
+      </c>
+      <c r="E10" s="28">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F10" s="28">
+        <v>17.5</v>
+      </c>
+      <c r="G10" s="28">
+        <v>17.8</v>
+      </c>
       <c r="N10" s="3" t="s">
         <v>35</v>
       </c>
@@ -1739,18 +1769,29 @@
         <v>26.42200729854547</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="A11" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="4">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="D11" s="30">
+        <v>13.8351376727394</v>
+      </c>
+      <c r="E11" s="30">
+        <v>16.144174311321741</v>
+      </c>
+      <c r="F11" s="30">
+        <v>18.337292879637591</v>
+      </c>
+      <c r="G11" s="30">
+        <v>19.939806622189707</v>
+      </c>
+      <c r="I11">
+        <f>G13*(G7/10^6+G11)+C12*(C11+C4)</f>
+        <v>17.8</v>
+      </c>
       <c r="N11" s="3" t="s">
         <v>36</v>
       </c>
@@ -1774,23 +1815,18 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" s="32">
+        <f>C10/(C4+C11)</f>
+        <v>4.7038795806827342E-2</v>
+      </c>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
       <c r="N12" s="3" t="s">
         <v>37</v>
       </c>
@@ -1813,23 +1849,26 @@
         <v>4.6709789600000002</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="21"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="27">
-        <v>137.54</v>
-      </c>
-      <c r="D13" s="27">
-        <v>165.75</v>
-      </c>
-      <c r="E13" s="27">
-        <v>172.9</v>
-      </c>
-      <c r="F13" s="27">
-        <v>179.8</v>
-      </c>
-      <c r="G13" s="27">
-        <v>183.9</v>
+    <row r="13" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32">
+        <f>(D10-$C$10)/(D7/10^6+D11)</f>
+        <v>0.1272338176991169</v>
+      </c>
+      <c r="E13" s="32">
+        <f t="shared" ref="E13:G13" si="2">(E10-$C$10)/(E7/10^6+E11)</f>
+        <v>0.11037864601385293</v>
+      </c>
+      <c r="F13" s="32">
+        <f t="shared" si="2"/>
+        <v>9.5671162954125061E-2</v>
+      </c>
+      <c r="G13" s="32">
+        <f t="shared" si="2"/>
+        <v>8.8603193760063065E-2</v>
       </c>
       <c r="N13" s="3" t="s">
         <v>38</v>
@@ -1853,14 +1892,16 @@
         <v>8.5676397800000004</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
+    <row r="14" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="18"/>
       <c r="N14" s="3" t="s">
         <v>39</v>
       </c>
@@ -1883,30 +1924,18 @@
         <v>24.178772760488858</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="7">
-        <v>0</v>
-      </c>
-      <c r="D15" s="7">
-        <f>75*$C$25*(1-$C$29)*$C$27*0.3</f>
-        <v>3.7084942228242932</v>
-      </c>
-      <c r="E15" s="7">
-        <f>75*$C$25*(1-$C$29)*$C$27*0.5</f>
-        <v>6.1808237047071559</v>
-      </c>
-      <c r="F15" s="7">
-        <f>75*$C$25*(1-$C$29)*$C$27*0.8</f>
-        <v>9.8893179275314509</v>
-      </c>
-      <c r="G15" s="7">
-        <f>75*$C$25*(1-$C$29)*$C$27*1</f>
-        <v>12.361647409414312</v>
-      </c>
+    <row r="15" spans="1:20" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="26"/>
       <c r="N15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1930,220 +1959,266 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="21"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P16" s="12">
+        <v>7.0940057399999992</v>
+      </c>
+      <c r="Q16" s="12">
+        <v>7.0940057399999992</v>
+      </c>
+      <c r="R16" s="12">
+        <v>7.0940057399999992</v>
+      </c>
+      <c r="S16" s="12">
+        <v>7.0940057399999992</v>
+      </c>
+      <c r="T16" s="12">
+        <v>7.0940057399999992</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="21"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="27">
+        <v>137.54</v>
+      </c>
+      <c r="D17" s="27">
+        <v>165.75</v>
+      </c>
+      <c r="E17" s="27">
+        <v>172.9</v>
+      </c>
+      <c r="F17" s="27">
+        <v>179.8</v>
+      </c>
+      <c r="G17" s="27">
+        <v>183.9</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P17" s="12">
+        <v>0.36178175000000001</v>
+      </c>
+      <c r="Q17" s="12">
+        <v>0.36178175000000001</v>
+      </c>
+      <c r="R17" s="12">
+        <v>0.36178175000000001</v>
+      </c>
+      <c r="S17" s="12">
+        <v>0.36178175000000001</v>
+      </c>
+      <c r="T17" s="12">
+        <v>0.36178175000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="N18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="12">
+        <v>54.302358825637938</v>
+      </c>
+      <c r="R18" s="12">
+        <v>54.302358825637903</v>
+      </c>
+      <c r="S18" s="12">
+        <v>54.302358825637938</v>
+      </c>
+      <c r="T18" s="12">
+        <v>54.302358825637938</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0</v>
+      </c>
+      <c r="D19" s="7">
+        <f>75*$C$31*(1-$C$35)*$C$33*0.3</f>
+        <v>3.7084942228242932</v>
+      </c>
+      <c r="E19" s="7">
+        <f>75*$C$31*(1-$C$35)*$C$33*0.5</f>
+        <v>6.1808237047071559</v>
+      </c>
+      <c r="F19" s="7">
+        <f>75*$C$31*(1-$C$35)*$C$33*0.8</f>
+        <v>9.8893179275314509</v>
+      </c>
+      <c r="G19" s="7">
+        <f>75*$C$31*(1-$C$35)*$C$33*1</f>
+        <v>12.361647409414312</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="12">
+        <v>0.33476888100000002</v>
+      </c>
+      <c r="R19" s="12">
+        <v>0.55794813499999985</v>
+      </c>
+      <c r="S19" s="12">
+        <v>0.89271701600000009</v>
+      </c>
+      <c r="T19" s="12">
+        <v>1.1158962699999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7">
-        <f>(D13-$C$13)*10^6</f>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7">
+        <f>(D17-$C$17)*10^6</f>
         <v>28210000.000000007</v>
       </c>
-      <c r="E16" s="7">
-        <f t="shared" ref="E16:G16" si="3">(E13-$C$13)*10^6</f>
+      <c r="E20" s="7">
+        <f t="shared" ref="E20:G20" si="3">(E17-$C$17)*10^6</f>
         <v>35360000.000000015</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F20" s="7">
         <f t="shared" si="3"/>
         <v>42260000.000000022</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G20" s="7">
         <f t="shared" si="3"/>
         <v>46360000.000000015</v>
       </c>
-      <c r="N16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="P16" s="12">
-        <v>7.0940057399999992</v>
-      </c>
-      <c r="Q16" s="12">
-        <v>7.0940057399999992</v>
-      </c>
-      <c r="R16" s="12">
-        <v>7.0940057399999992</v>
-      </c>
-      <c r="S16" s="12">
-        <v>7.0940057399999992</v>
-      </c>
-      <c r="T16" s="12">
-        <v>7.0940057399999992</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B17" s="7" t="s">
+      <c r="N20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P20" s="12">
+        <v>40368.159200000002</v>
+      </c>
+      <c r="Q20" s="12">
+        <v>40368.159200000002</v>
+      </c>
+      <c r="R20" s="12">
+        <v>40368.159200000002</v>
+      </c>
+      <c r="S20" s="12">
+        <v>40368.159200000002</v>
+      </c>
+      <c r="T20" s="12">
+        <v>40368.159200000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7">
-        <f>D16/D15</f>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7">
+        <f>D20/D19</f>
         <v>7606860.9804968229</v>
       </c>
-      <c r="E17" s="7">
-        <f t="shared" ref="E17" si="4">E16/E15</f>
+      <c r="E21" s="7">
+        <f t="shared" ref="E21" si="4">E20/E19</f>
         <v>5720920.331875952</v>
       </c>
-      <c r="F17" s="7">
-        <f>F16/F15</f>
+      <c r="F21" s="7">
+        <f>F20/F19</f>
         <v>4273297.7450699545</v>
       </c>
-      <c r="G17" s="7">
-        <f t="shared" ref="G17" si="5">G16/G15</f>
+      <c r="G21" s="7">
+        <f t="shared" ref="G21" si="5">G20/G19</f>
         <v>3750309.1994594052</v>
       </c>
-      <c r="N17" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="P17" s="12">
-        <v>0.36178175000000001</v>
-      </c>
-      <c r="Q17" s="12">
-        <v>0.36178175000000001</v>
-      </c>
-      <c r="R17" s="12">
-        <v>0.36178175000000001</v>
-      </c>
-      <c r="S17" s="12">
-        <v>0.36178175000000001</v>
-      </c>
-      <c r="T17" s="12">
-        <v>0.36178175000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="N21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="P21" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="12">
+        <v>-33.114527371853342</v>
+      </c>
+      <c r="R21" s="12">
+        <v>-28.278772819755574</v>
+      </c>
+      <c r="S21" s="12">
+        <v>-21.025140991608914</v>
+      </c>
+      <c r="T21" s="12">
+        <v>-16.189386439511143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="D18">
-        <f>D17/10^6</f>
+      <c r="D22">
+        <f>D21/10^6</f>
         <v>7.6068609804968226</v>
       </c>
-      <c r="E18">
-        <f t="shared" ref="E18:G18" si="6">E17/10^6</f>
+      <c r="E22">
+        <f t="shared" ref="E22:G22" si="6">E21/10^6</f>
         <v>5.7209203318759521</v>
       </c>
-      <c r="F18">
+      <c r="F22">
         <f t="shared" si="6"/>
         <v>4.2732977450699545</v>
       </c>
-      <c r="G18">
+      <c r="G22">
         <f t="shared" si="6"/>
         <v>3.7503091994594051</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q18" s="12">
-        <v>54.302358825637938</v>
-      </c>
-      <c r="R18" s="12">
-        <v>54.302358825637903</v>
-      </c>
-      <c r="S18" s="12">
-        <v>54.302358825637938</v>
-      </c>
-      <c r="T18" s="12">
-        <v>54.302358825637938</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="N19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="O19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="P19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q19" s="12">
-        <v>0.33476888100000002</v>
-      </c>
-      <c r="R19" s="12">
-        <v>0.55794813499999985</v>
-      </c>
-      <c r="S19" s="12">
-        <v>0.89271701600000009</v>
-      </c>
-      <c r="T19" s="12">
-        <v>1.1158962699999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="N20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="P20" s="12">
-        <v>40368.159200000002</v>
-      </c>
-      <c r="Q20" s="12">
-        <v>40368.159200000002</v>
-      </c>
-      <c r="R20" s="12">
-        <v>40368.159200000002</v>
-      </c>
-      <c r="S20" s="12">
-        <v>40368.159200000002</v>
-      </c>
-      <c r="T20" s="12">
-        <v>40368.159200000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0.95</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O21" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="P21" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="12">
-        <v>-33.114527371853342</v>
-      </c>
-      <c r="R21" s="12">
-        <v>-28.278772819755574</v>
-      </c>
-      <c r="S21" s="12">
-        <v>-21.025140991608914</v>
-      </c>
-      <c r="T21" s="12">
-        <v>-16.189386439511143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="9">
-        <v>0.79249999999999998</v>
       </c>
       <c r="N22" s="3"/>
       <c r="O22" s="12"/>
@@ -2162,22 +2237,23 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="B23" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="E23">
-        <f>C23*(1-0.95)</f>
-        <v>4.1650000000000034E-2</v>
-      </c>
-      <c r="G23">
-        <f>0.95/(1+C24)</f>
-        <v>0.88219474555148414</v>
+        <v>68</v>
+      </c>
+      <c r="C23" s="28">
+        <v>9.68</v>
+      </c>
+      <c r="D23" s="28">
+        <v>15</v>
+      </c>
+      <c r="E23" s="28">
+        <v>15.3</v>
+      </c>
+      <c r="F23" s="28">
+        <v>15.5</v>
+      </c>
+      <c r="G23" s="28">
+        <v>15.7</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>51</v>
@@ -2202,15 +2278,27 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" s="6">
-        <f>P5/O4-1</f>
-        <v>7.6859735098658843E-2</v>
+      <c r="B24" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4">
+        <v>61</v>
+      </c>
+      <c r="D24" s="30">
+        <v>10.684945673991011</v>
+      </c>
+      <c r="E24" s="30">
+        <v>12.848498270378062</v>
+      </c>
+      <c r="F24" s="30">
+        <v>15.269676480302797</v>
+      </c>
+      <c r="G24" s="30">
+        <v>16.588739769484363</v>
+      </c>
+      <c r="I24">
+        <f>G26*(G20/10^6+G24)+$C$25*($C$24+$C$17)</f>
+        <v>15.7</v>
       </c>
       <c r="N24" s="3" t="s">
         <v>47</v>
@@ -2235,20 +2323,17 @@
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="B25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="7">
-        <f>C23*(1+C24)</f>
-        <v>0.89702415933718282</v>
-      </c>
-      <c r="E25">
-        <f>C25*(1-0.95)/(1+C24)</f>
-        <v>4.1650000000000034E-2</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C25" s="32">
+        <f>C23/(C17+C24)</f>
+        <v>4.8755918202881034E-2</v>
+      </c>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
       <c r="N25" s="3" t="s">
         <v>52</v>
       </c>
@@ -2272,19 +2357,25 @@
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="5">
-        <f>1/C21-(1-C21)/(C21*(1+C24))</f>
-        <v>1.0037565237921615</v>
-      </c>
-      <c r="E26">
-        <f>C25*(1-0.95*C26)</f>
-        <v>4.165000000000009E-2</v>
+      <c r="B26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32">
+        <f>(D23-$C$23)/(D20/10^6+D24)</f>
+        <v>0.13677869727833236</v>
+      </c>
+      <c r="E26" s="32">
+        <f t="shared" ref="E26:G26" si="7">(E23-$C$23)/(E20/10^6+E24)</f>
+        <v>0.11657695637976832</v>
+      </c>
+      <c r="F26" s="32">
+        <f t="shared" si="7"/>
+        <v>0.10116517867074516</v>
+      </c>
+      <c r="G26" s="32">
+        <f t="shared" si="7"/>
+        <v>9.5633368071306665E-2</v>
       </c>
       <c r="N26" s="3" t="s">
         <v>48</v>
@@ -2309,15 +2400,14 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="8">
-        <f>C21*C26</f>
-        <v>0.95356869760255336</v>
+      <c r="C27" s="9">
+        <v>0.95</v>
       </c>
       <c r="N27" s="3" t="s">
         <v>49</v>
@@ -2342,15 +2432,14 @@
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="5">
-        <f>1/C22-(1-C22)/(C22*(1+C24))</f>
-        <v>1.0186878170985447</v>
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0.79249999999999998</v>
       </c>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -2361,15 +2450,22 @@
       <c r="T28" s="3"/>
     </row>
     <row r="29" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" s="8">
-        <f>C22*C28</f>
-        <v>0.8073100950505967</v>
+      <c r="A29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="E29">
+        <f>C29*(1-0.95)</f>
+        <v>4.1650000000000034E-2</v>
+      </c>
+      <c r="G29">
+        <f>0.95/(1+C30)</f>
+        <v>0.88219474555148414</v>
       </c>
       <c r="N29" s="11"/>
       <c r="O29" s="11" t="s">
@@ -2382,6 +2478,16 @@
       <c r="T29" s="11"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="6">
+        <f>P5/O4-1</f>
+        <v>7.6859735098658843E-2</v>
+      </c>
       <c r="N30" s="3"/>
       <c r="O30" s="3" t="s">
         <v>27</v>
@@ -2403,6 +2509,20 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="7">
+        <f>C29*(1+C30)</f>
+        <v>0.89702415933718282</v>
+      </c>
+      <c r="E31">
+        <f>C31*(1-0.95)/(1+C30)</f>
+        <v>4.1650000000000034E-2</v>
+      </c>
       <c r="N31" s="3" t="s">
         <v>28</v>
       </c>
@@ -2426,15 +2546,19 @@
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32" s="7">
-        <f>AVERAGE(P51,P23)*1000/3600</f>
-        <v>0.25548249251013122</v>
+      <c r="A32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C32" s="5">
+        <f>1/C27-(1-C27)/(C27*(1+C30))</f>
+        <v>1.0037565237921615</v>
+      </c>
+      <c r="E32">
+        <f>C31*(1-0.95*C32)</f>
+        <v>4.165000000000009E-2</v>
       </c>
       <c r="N32" s="3" t="s">
         <v>29</v>
@@ -2459,15 +2583,15 @@
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C33" s="7">
-        <f>P25/1000</f>
-        <v>8.2307186539958971E-2</v>
+      <c r="A33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="8">
+        <f>C27*C32</f>
+        <v>0.95356869760255336</v>
       </c>
       <c r="N33" s="3" t="s">
         <v>30</v>
@@ -2492,15 +2616,15 @@
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="7">
-        <f>Q18/1000</f>
-        <v>5.4302358825637935E-2</v>
+      <c r="A34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="5">
+        <f>1/C28-(1-C28)/(C28*(1+C30))</f>
+        <v>1.0186878170985447</v>
       </c>
       <c r="N34" s="3" t="s">
         <v>31</v>
@@ -2525,6 +2649,16 @@
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="8">
+        <f>C28*C34</f>
+        <v>0.8073100950505967</v>
+      </c>
       <c r="N35" s="3" t="s">
         <v>32</v>
       </c>
@@ -2594,6 +2728,16 @@
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="7">
+        <f>AVERAGE(P51,P23)*1000/3600</f>
+        <v>0.25548249251013122</v>
+      </c>
       <c r="N38" s="3" t="s">
         <v>35</v>
       </c>
@@ -2617,6 +2761,16 @@
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="7">
+        <f>P25/1000</f>
+        <v>8.2307186539958971E-2</v>
+      </c>
       <c r="N39" s="3" t="s">
         <v>36</v>
       </c>
@@ -2640,6 +2794,16 @@
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C40" s="7">
+        <f>Q18/1000</f>
+        <v>5.4302358825637935E-2</v>
+      </c>
       <c r="N40" s="3" t="s">
         <v>37</v>
       </c>
@@ -2663,6 +2827,7 @@
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H41" s="13"/>
       <c r="N41" s="3" t="s">
         <v>38</v>
       </c>
@@ -2686,6 +2851,7 @@
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H42" s="13"/>
       <c r="N42" s="3" t="s">
         <v>39</v>
       </c>
@@ -2709,6 +2875,7 @@
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H43" s="13"/>
       <c r="N43" s="3" t="s">
         <v>40</v>
       </c>
@@ -2732,6 +2899,7 @@
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="H44" s="13"/>
       <c r="N44" s="3" t="s">
         <v>41</v>
       </c>
@@ -2755,6 +2923,13 @@
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B45" s="13"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="13"/>
       <c r="N45" s="3" t="s">
         <v>42</v>
       </c>
@@ -2778,6 +2953,13 @@
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B46" s="13"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="13"/>
       <c r="N46" s="3" t="s">
         <v>43</v>
       </c>
@@ -2801,6 +2983,13 @@
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
       <c r="N47" s="3" t="s">
         <v>44</v>
       </c>
@@ -2824,6 +3013,13 @@
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
       <c r="N48" s="3" t="s">
         <v>45</v>
       </c>
@@ -2846,7 +3042,13 @@
         <v>23737.731500000002</v>
       </c>
     </row>
-    <row r="49" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
       <c r="N49" s="3" t="s">
         <v>46</v>
       </c>
@@ -2869,7 +3071,13 @@
         <v>-9.1644977901038853</v>
       </c>
     </row>
-    <row r="50" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B50" s="13"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
       <c r="N50" s="3"/>
       <c r="O50" s="12"/>
       <c r="P50" s="12"/>
@@ -2886,7 +3094,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
       <c r="N51" s="3" t="s">
         <v>51</v>
       </c>
@@ -2909,7 +3123,13 @@
         <v>0.74863011783778244</v>
       </c>
     </row>
-    <row r="52" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
       <c r="N52" s="3" t="s">
         <v>47</v>
       </c>
@@ -2932,7 +3152,7 @@
         <v>4425.9421357692881</v>
       </c>
     </row>
-    <row r="53" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N53" s="3" t="s">
         <v>52</v>
       </c>
@@ -2955,7 +3175,7 @@
         <v>66.346218081835687</v>
       </c>
     </row>
-    <row r="54" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N54" s="3" t="s">
         <v>48</v>
       </c>
@@ -2978,7 +3198,7 @@
         <v>8.4360410255996303</v>
       </c>
     </row>
-    <row r="55" spans="14:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:20" x14ac:dyDescent="0.3">
       <c r="N55" s="3" t="s">
         <v>49</v>
       </c>
@@ -3003,6 +3223,14 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A14:G14"/>
+    <mergeCell ref="A15:B18"/>
+    <mergeCell ref="C15:G15"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:B5"/>
     <mergeCell ref="C2:G2"/>
@@ -3011,14 +3239,6 @@
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:B14"/>
-    <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>